<commit_message>
More work on mansucript
</commit_message>
<xml_diff>
--- a/R_output_files/Tables/Moiety_Statistics_Table.xlsx
+++ b/R_output_files/Tables/Moiety_Statistics_Table.xlsx
@@ -381,10 +381,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>37.60532541702649</v>
+        <v>37.6319425138707</v>
       </c>
       <c r="C2">
-        <v>0.7244974994633325</v>
+        <v>0.7360327430743545</v>
       </c>
     </row>
     <row r="3">
@@ -394,10 +394,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>45.52748874112216</v>
+        <v>45.57433487359113</v>
       </c>
       <c r="C3">
-        <v>1.353977359119062</v>
+        <v>1.340339211219409</v>
       </c>
     </row>
     <row r="4">
@@ -407,10 +407,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>14.51528478570747</v>
+        <v>14.51641272179008</v>
       </c>
       <c r="C4">
-        <v>1.840823395850111</v>
+        <v>1.840780798059799</v>
       </c>
     </row>
     <row r="5">
@@ -446,10 +446,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.07459116539580023</v>
+        <v>0.0978797837110706</v>
       </c>
       <c r="C7">
-        <v>0.05933824740560668</v>
+        <v>0.08012049418058301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>